<commit_message>
Covfefe 5: the search is not over
</commit_message>
<xml_diff>
--- a/TP1/Punto 2/Mediciones.xlsx
+++ b/TP1/Punto 2/Mediciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellon\source\repos\TC\TP1\Punto 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B188D2-8A45-4168-B8C6-DC9B82F3BB73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACDE4C0-8E8E-4B6D-AE98-31D3A1FD01D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{555DA7CC-7A38-4795-B3ED-2A85C07D66EC}"/>
   </bookViews>
@@ -43,10 +43,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00000000000"/>
-    <numFmt numFmtId="181" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -119,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,13 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -146,20 +141,32 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -345,6 +352,9 @@
                 <c:pt idx="23">
                   <c:v>480000</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>4800000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -352,7 +362,7 @@
             <c:numRef>
               <c:f>'Ejercicio 2'!$B$2:$B$32</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="1">
                   <c:v>-0.1</c:v>
@@ -386,6 +396,48 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-12.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-13.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-14.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-15.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-16.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-17.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-17.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-18.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-18.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-19.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-19.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,6 +588,9 @@
                       </c:pt>
                       <c:pt idx="23">
                         <c:v>480000</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>4800000</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1303,16 +1358,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1640,7 +1695,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A27" sqref="A27:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,10 +1708,10 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="10"/>
       <c r="D1">
         <f>(480-4.8)*1000/20</f>
         <v>23760</v>
@@ -1665,12 +1720,12 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="10"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3" s="11">
         <v>1000</v>
       </c>
       <c r="B3" s="14">
@@ -1680,7 +1735,7 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="11">
         <v>2000</v>
       </c>
       <c r="B4" s="14">
@@ -1690,27 +1745,27 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="11">
         <f>4.8*1000</f>
         <v>4800</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="15">
         <v>-0.1</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="11">
         <f>A5+$D$1</f>
         <v>28560</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="15">
         <v>-1.8</v>
       </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="11">
         <v>48000</v>
       </c>
       <c r="B7" s="14">
@@ -1719,261 +1774,291 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="11">
         <f>A6+$D$1</f>
         <v>52320</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="15">
         <v>-4.5</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <f>A8+$D$1</f>
+      <c r="A9" s="11">
+        <f t="shared" ref="A9:A26" si="0">A8+$D$1</f>
         <v>76080</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="15">
         <v>-6.4</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
-        <f>A9+$D$1</f>
+      <c r="A10" s="11">
+        <f t="shared" si="0"/>
         <v>99840</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="15">
         <v>-8.1999999999999993</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <f>A10+$D$1</f>
+      <c r="A11" s="11">
+        <f t="shared" si="0"/>
         <v>123600</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="15">
         <v>-9.6</v>
       </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <f>A11+$D$1</f>
+      <c r="A12" s="11">
+        <f t="shared" si="0"/>
         <v>147360</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="15">
         <v>-10.9</v>
       </c>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <f>A12+$D$1</f>
+      <c r="A13" s="11">
+        <f t="shared" si="0"/>
         <v>171120</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="15">
         <v>-12</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <f>A13+$D$1</f>
+      <c r="A14" s="11">
+        <f t="shared" si="0"/>
         <v>194880</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="15">
+        <v>-12.9</v>
+      </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
-        <f>A14+$D$1</f>
+      <c r="A15" s="11">
+        <f t="shared" si="0"/>
         <v>218640</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="15">
+        <v>-13.8</v>
+      </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
-        <f>A15+$D$1</f>
+      <c r="A16" s="11">
+        <f t="shared" si="0"/>
         <v>242400</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="15">
+        <v>-14.6</v>
+      </c>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
-        <f>A16+$D$1</f>
+      <c r="A17" s="11">
+        <f t="shared" si="0"/>
         <v>266160</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="15">
+        <v>-15.4</v>
+      </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
-        <f>A17+$D$1</f>
+      <c r="A18" s="11">
+        <f t="shared" si="0"/>
         <v>289920</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="15">
+        <v>-16</v>
+      </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <f>A18+$D$1</f>
+      <c r="A19" s="11">
+        <f t="shared" si="0"/>
         <v>313680</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="15">
+        <v>-16.7</v>
+      </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
-        <f>A19+$D$1</f>
+      <c r="A20" s="11">
+        <f t="shared" si="0"/>
         <v>337440</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="15">
+        <v>-17.2</v>
+      </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
-        <f>A20+$D$1</f>
+      <c r="A21" s="11">
+        <f t="shared" si="0"/>
         <v>361200</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="15">
+        <v>-17.8</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <f>A21+$D$1</f>
+      <c r="A22" s="11">
+        <f t="shared" si="0"/>
         <v>384960</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="15">
+        <v>-18.3</v>
+      </c>
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
-        <f>A22+$D$1</f>
+      <c r="A23" s="11">
+        <f t="shared" si="0"/>
         <v>408720</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="15">
+        <v>-18.7</v>
+      </c>
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
-        <f>A23+$D$1</f>
+      <c r="A24" s="11">
+        <f t="shared" si="0"/>
         <v>432480</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="15">
+        <v>-19.3</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
-        <f>A24+$D$1</f>
+      <c r="A25" s="11">
+        <f t="shared" si="0"/>
         <v>456240</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="15">
+        <v>-19.600000000000001</v>
+      </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
-        <f>A25+$D$1</f>
+      <c r="A26" s="11">
+        <f t="shared" si="0"/>
         <v>480000</v>
       </c>
-      <c r="B26" s="6"/>
+      <c r="B26" s="15">
+        <v>-20</v>
+      </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="19">
+        <v>4800000</v>
+      </c>
+      <c r="B27" s="15">
+        <v>-30</v>
+      </c>
       <c r="C27" s="5"/>
-      <c r="I27" s="8"/>
+      <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="11"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="11"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="11"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="11"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="11"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="11"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>